<commit_message>
edit file lược đồ,sửa SRS,sửa file test case
</commit_message>
<xml_diff>
--- a/Lending/Document/UIUX.U39_CustomRetailUsers_action_init.xlsx
+++ b/Lending/Document/UIUX.U39_CustomRetailUsers_action_init.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TaiLieu\UIUXIBMB-29_getCardDetail_OCBOut\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspaces_2018\DemoSAP_UI5_Git\SAPUI_DEMO\Lending\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34E79F9D-52B1-4B50-8148-068AD0040526}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7095"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Testcase" sheetId="2" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t>TT</t>
   </si>
@@ -106,94 +107,106 @@
     <t>System</t>
   </si>
   <si>
-    <t>tuancmq</t>
-  </si>
-  <si>
-    <t>IIB</t>
-  </si>
-  <si>
     <t>Bắn thử meessage thành công</t>
   </si>
   <si>
     <t>Bắn thử message thành công</t>
   </si>
   <si>
-    <t>OCBOut_getCardDetail</t>
-  </si>
-  <si>
-    <t>getCardDetail</t>
-  </si>
-  <si>
-    <t>&lt;soapenv:Envelope xmlns:soapenv="http://schemas.xmlsoap.org/soap/envelope/"&gt;
-   &lt;soapenv:Body&gt;
-      &lt;ocb:getCardDetailRs xmlns:ocb="http://www.vpbank.com.vn/ASBOOCBOut"&gt;
-         &lt;responseStatus&gt;
-            &lt;resultCode&gt;0&lt;/resultCode&gt;
-         &lt;/responseStatus&gt;
-         &lt;cardInfo&gt;
-            &lt;id&gt;6694666&lt;/id&gt;
-            &lt;number&gt;5203993010928562&lt;/number&gt;
-            &lt;type&gt;CC&lt;/type&gt;
-            &lt;maskNumber&gt;520399______8562&lt;/maskNumber&gt;
-            &lt;branchNo&gt;VN0010325&lt;/branchNo&gt;
-            &lt;interestRate&gt;44&lt;/interestRate&gt;
-            &lt;holderName&gt;HOANG  ANH TUAN&lt;/holderName&gt;
-            &lt;status&gt;Card De-active&lt;/status&gt;
-            &lt;plasticStatus&gt;To Close&lt;/plasticStatus&gt;
-            &lt;EComStatus&gt;Active&lt;/EComStatus&gt;
-            &lt;activeDate/&gt;
-            &lt;unlockDate/&gt;
-            &lt;openDate&gt;23/05/2016&lt;/openDate&gt;
-            &lt;shortName&gt;HOANG  ANH TUAN&lt;/shortName&gt;
-            &lt;regNumber&gt;014671875298&lt;/regNumber&gt;
-            &lt;clientNumber&gt;3770120&lt;/clientNumber&gt;
-            &lt;stmtDate&gt;6&lt;/stmtDate&gt;
-            &lt;stmtProductName&gt;MC2 Credit&lt;/stmtProductName&gt;
-            &lt;currency&gt;VND&lt;/currency&gt;
-            &lt;contractNumber&gt;325-P-326091&lt;/contractNumber&gt;
-            &lt;validThrough&gt;2105&lt;/validThrough&gt;
-            &lt;cardType&gt;Credit&lt;/cardType&gt;
-         &lt;/cardInfo&gt;
-         &lt;productInfo&gt;
-            &lt;id&gt;ISSMCSC&lt;/id&gt;
-            &lt;type&gt;prin&lt;/type&gt;
-            &lt;code&gt;MSCO&lt;/code&gt;
-            &lt;name&gt;MC2 Credit Orange&lt;/name&gt;
-            &lt;groupName&gt;Issuing MC2 Credit&lt;/groupName&gt;
-         &lt;/productInfo&gt;
-         &lt;balanceInfo&gt;
-            &lt;creditLimit&gt;-10000000&lt;/creditLimit&gt;
-            &lt;availableBalance&gt;56802989.96&lt;/availableBalance&gt;
-            &lt;blockAmount&gt;-54946937&lt;/blockAmount&gt;
-            &lt;cardBalance&gt;-8143947.04&lt;/cardBalance&gt;
-            &lt;totalAmount&gt;-8143947.04&lt;/totalAmount&gt;
-            &lt;minimumPayDue&gt;0&lt;/minimumPayDue&gt;
-            &lt;outstandingAmount&gt;-8143948&lt;/outstandingAmount&gt;
-         &lt;/balanceInfo&gt;
-      &lt;/ocb:getCardDetailRs&gt;
-   &lt;/soapenv:Body&gt;
-&lt;/soapenv:Envelope&gt;</t>
-  </si>
-  <si>
-    <t>&lt;soapenv:Envelope xmlns:soapenv="http://schemas.xmlsoap.org/soap/envelope/" xmlns:asb="http://www.vpbank.com.vn/ASBOOCBOut"&gt;
-   &lt;soapenv:Header/&gt;
-   &lt;soapenv:Body&gt;
-      &lt;asb:getCardDetailRq sessionId="abc123"&gt;
-         &lt;cardNo&gt;5203993010928562&lt;/cardNo&gt;
-      &lt;/asb:getCardDetailRq&gt;
-   &lt;/soapenv:Body&gt;
-&lt;/soapenv:Envelope&gt;</t>
+    <t>khoand</t>
+  </si>
+  <si>
+    <t>OCB</t>
+  </si>
+  <si>
+    <t>CustomRetailUsers_action=init</t>
+  </si>
+  <si>
+    <t>{
+    "d": {
+        "__metadata": {
+            "id": "https://smp-srv:8081/cb/odata/services/retailuserservice/CustomRetailUsers('469')",
+            "uri": "https://smp-srv:8081/cb/odata/services/retailuserservice/CustomRetailUsers('469')",
+            "type": "com.sap.banking.custom.user.endpoint.v1_0.beans.CustomRetailUser"
+        },
+        "Id": "469",
+        "FirstName": "none",
+        "LastName": "VPBANK469",
+        "MiddleName": null,
+        "AffiliateBankID": 1,
+        "BankId": "1000",
+        "ConfirmPassword": null,
+        "ConfirmPasswordReminder": null,
+        "ConfirmPasswordReminder2": null,
+        "CustId": "884206",
+        "Greeting": null,
+        "GreetingType": "1",
+        "Password": "FFIHASHKXsZIfopn7b7u3sxzB6LbWJ5HLZfMhmAE+UhiJcCZKo=",
+        "PasswordClue": "What is your favorite food?",
+        "PasswordClue2": "What is your favorite movie?",
+        "MemberId": null,
+        "GroupId": "2139",
+        "GroupName": null,
+        "PasswordReminder": null,
+        "PasswordReminder2": null,
+        "PersonalBanker": "0",
+        "Ssn": null,
+        "MaskSSN": "",
+        "UserName": "namnguyen",
+        "AccountStatus": "1",
+        "Timeout": "300",
+        "CustomerType": "2",
+        "RequestedCarrierTCId": null,
+        "Address": {
+            "__metadata": {
+                "type": "com.sap.banking.common.endpoint.v1_0.beans.Address"
+            },
+            "Street": "VPBANK469",
+            "Street2": "VPBANK469",
+            "Street3": null,
+            "City": null,
+            "State": null,
+            "StreetCode": null,
+            "Country": "VNM",
+            "Email": "tienthanhle38@gmail.com",
+            "Phone": "03495896391",
+            "Phone2": "VPBANK469",
+            "ZipCode": null,
+            "DataPhone": "0383962087",
+            "FaxPhone": null,
+            "PreferredContactMethod": null,
+            "PreferredLanguage": "en_US"
+        },
+        "OldPassword": null,
+        "NewPassword": null,
+        "OldOtpMethod": "2",
+        "NewOtpMethod": null,
+        "OldServicePackage": "200000012",
+        "OldServicePackageName": "PLATINIUM",
+        "NewServicePackage": null,
+        "NewServicePackageName": null,
+        "ServicePackages": "200000010#INQUIRY;200000011#STANDARD",
+        "Transactions": {
+            "__deferred": {
+                "uri": "https://smp-srv:8081/cb/odata/services/retailuserservice/CustomRetailUsers('469')/Transactions"
+            }
+        }
+    }
+}</t>
+  </si>
+  <si>
+    <t>https://smp-srv:8081/cb/odata/services/retailuserservice/CustomRetailUsers('469')?action=init</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -201,7 +214,7 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -210,7 +223,7 @@
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -219,7 +232,7 @@
       <b/>
       <sz val="9"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -246,7 +259,7 @@
       <i/>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -263,14 +276,6 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="163"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -395,9 +400,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -436,6 +438,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -500,7 +505,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 4" descr="C:\Users\LANLH\Pictures\New logo.jpg"/>
+        <xdr:cNvPr id="2" name="Picture 4" descr="C:\Users\LANLH\Pictures\New logo.jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -818,47 +829,47 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A4:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" customWidth="1"/>
+    <col min="1" max="1" width="7.8984375" customWidth="1"/>
+    <col min="2" max="2" width="23.296875" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="4" width="7.140625" customWidth="1"/>
+    <col min="4" max="4" width="7.09765625" customWidth="1"/>
     <col min="5" max="5" width="24" customWidth="1"/>
-    <col min="6" max="6" width="47.85546875" customWidth="1"/>
-    <col min="7" max="7" width="20.7109375" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" customWidth="1"/>
-    <col min="9" max="9" width="27.85546875" customWidth="1"/>
+    <col min="6" max="6" width="47.8984375" customWidth="1"/>
+    <col min="7" max="7" width="20.69921875" customWidth="1"/>
+    <col min="8" max="8" width="10.3984375" customWidth="1"/>
+    <col min="9" max="9" width="27.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:11" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+    <row r="4" spans="1:11" ht="34.799999999999997" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
     </row>
     <row r="5" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="13" t="s">
         <v>21</v>
       </c>
     </row>
@@ -879,7 +890,7 @@
         <v>14</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -887,81 +898,81 @@
         <v>16</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="22" t="s">
+      <c r="C12" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="17" t="s">
+      <c r="E12" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="17" t="s">
+      <c r="F12" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="G12" s="17" t="s">
+      <c r="G12" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="H12" s="22" t="s">
+      <c r="H12" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="I12" s="22" t="s">
+      <c r="I12" s="21" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="20"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="22"/>
+      <c r="A13" s="19"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="21"/>
-      <c r="B14" s="22"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="22"/>
+      <c r="A14" s="20"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
     </row>
     <row r="15" spans="1:11" ht="270" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>1</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="F15" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>3</v>
@@ -979,10 +990,10 @@
         <v>12</v>
       </c>
       <c r="C17" s="8"/>
-      <c r="G17" s="16" t="s">
+      <c r="G17" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="H17" s="16"/>
+      <c r="H17" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="11">

</xml_diff>